<commit_message>
add cyberagent model test
</commit_message>
<xml_diff>
--- a/model_test/result/all_models_results.xlsx
+++ b/model_test/result/all_models_results.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YShimada-MBP16/Documents/Code_Github/LLM/model_test/result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E09ACBD-334E-9F43-806A-8D4CF97DD16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF9CEAC-7D60-0E43-A8D3-48174A000018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37340" yWindow="1040" windowWidth="27900" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38300" yWindow="3200" windowWidth="29260" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="res_JapaneseQuizChatbot_v1" sheetId="1" r:id="rId1"/>
+    <sheet name="結果" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="137">
   <si>
     <t>no</t>
   </si>
@@ -429,12 +431,159 @@
     <t>yukismd/JapaneseQuizChatbot_v1 による回答</t>
     <phoneticPr fontId="18"/>
   </si>
+  <si>
+    <t>ChatGPT (GPT-3.5) 正誤</t>
+    <rPh sb="18" eb="20">
+      <t xml:space="preserve">セイゴ </t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>yukismd/JapaneseQuizChatbot_v1 正誤</t>
+    <rPh sb="31" eb="33">
+      <t xml:space="preserve">セイゴ </t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>×</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>△</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>「走り幅跳び」です。なぜだと思いますか?それは、「走る」「跳ぶ」という二つの動作を連続的に行わなければならないからです。つまり「速さ」と「強さ」の両方が必要な種目なんです。そして、両方を同時にこなすには、スピードよりも強さが大切になります。そのため、最初に「速</t>
+  </si>
+  <si>
+    <t>正解は...埼玉県。県庁所在地である大宮市の市木は「サクラ」、市町村合併で誕生した三芳町では、「サツキ」です。また、西埼玉の中央部にあたる入間市と日高市に跨る狭山茶の主産地、所沢市では「ケヤキ」が主役となっています。そして、県立</t>
+  </si>
+  <si>
+    <t>ドイツ。1994年リレハンメル冬季オリンピックの男子シングルで、当時18歳だった彼は4位入賞を果たした。その直後に行われた世界選手権では、ショートプログラムで2位、フリーでは5位と健闘した。そして、翌年の長野オリンピックでは見事に金メダルを獲得。彼の名前を一躍世界に知らしめた。ちなみに彼が師事していた</t>
+  </si>
+  <si>
+    <t> シャッターとスプーン。シャッタストローはフランス語では「saute」で、「すくい取る・押しつぶす」といった意味があります。スプーンは英語では「spoon」。</t>
+  </si>
+  <si>
+    <t>バターは、乳脂肪分80%以上。マーガリンは、油脂を硬化させて作った食品で、含有量はおよそ60%。どちらも風味の面から『バターやマーガリン』と表記されています。どちらを選ぶかは好みですが、最近ではコレステロールやトランス脂肪酸、カロリーといった健康面からも注目されており、バター</t>
+  </si>
+  <si>
+    <t> 日本人の「武士道精神」の表れ。</t>
+  </si>
+  <si>
+    <t>「電力と効率の関係を表す式」です。電力を供給する側、つまり発電側は「単位時間あたりの電気エネルギー量」(すなわち発電した分)をワットWで表し、一方受電側の需要家は「単位時間当たりの利用可能容量」(すなわち使える電気の量)をアンペアAで</t>
+  </si>
+  <si>
+    <t>「蟹工船」です。この「蟹工船」は、いわゆる『蟹工船』の文庫版であり、今現在はもう手に入らないと思いますが、『蟹工船・党生活者』(角川書店)に収録されているものです。この本は岩波現代文庫にも収録されていますが、表紙が違うのです。『蟹工船</t>
+  </si>
+  <si>
+    <t>答えの予想は「ヘリウム」です。ただ、宇宙全体を考えると、重さも光速も時間すら無限大ということから、数えられる限りの元素やエネルギーの総量(質量×長さ)は無限大ということになります。つまり、未知の素粒子・エネルギーの塊であり、人類にとって未知の存在である</t>
+  </si>
+  <si>
+    <t>ペニシリウム属カビの一種から発見された「ペニシリン」という抗菌薬。細菌の細胞壁の合成を阻害する作用があり、特に肺炎球菌やインフルエンザ菌などに効果を発揮した。日本では1953年に製造販売承認され、1967年までに825万人の命を救ったと言われている。</t>
+  </si>
+  <si>
+    <t>「ね」で終わる。つまり、根津(ねづ)である。</t>
+  </si>
+  <si>
+    <t>「日本海」と答える人がほとんどです。ではなぜ「日本海」と言うのか。それは、「東海」「日本海」「東シナ海」「南海」の4つの言葉がすべて漢字で書けるからです。「西と東から来るもの」= 「東西南北」(日本語は世界で一番長い言葉)という発想があるようです。そして日本は</t>
+  </si>
+  <si>
+    <t>「英語」です。そして、彼女にはある秘密があります...。
+それでは解答...担当は国語でした。しかし、「数学」「歴史」も大事ですよね!</t>
+  </si>
+  <si>
+    <t>「英語」です。そして、彼女にはある秘密があります...。
+それでは解答...担当は国語でした。しかし、「数学」「歴史」も大事ですよね!</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>品川区です。
+2020.02.18更新
+2月16日~3月22日までの期間、東京都ではコロナウイルス感染症の緊急事態宣言が出されています。そこで当院では下記のような対応をさせていただくことにしました。尚、状況に応じて随時変更の可能性がありますことをご了承願います。そしてご来院の際はマスク着用をお願いいたします。発熱・咳</t>
+  </si>
+  <si>
+    <t>品川区です。
+2020.02.18更新
+2月16日~3月22日までの期間、東京都ではコロナウイルス感染症の緊急事態宣言が出されています。そこで当院では下記のような対応をさせていただくことにしました。尚、状況に応じて随時変更の可能性がありますことをご了承願います。そしてご来院の際はマスク着用をお願いいたします。発熱・咳</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>「肝臓」。肝細胞は傷ついても修復される再生能力がある。
+【答え】クイズは以上です。【解説】脂肪肝や肝炎、肝硬変などは、生活習慣から生じる生活習慣病であり、アルコール性・非アルコール性のいずれにも見られる。近年、肥満に伴うメタボリック症候群が注目されているが、過</t>
+  </si>
+  <si>
+    <t>「肝臓」。肝細胞は傷ついても修復される再生能力がある。
+【答え】クイズは以上です。【解説】脂肪肝や肝炎、肝硬変などは、生活習慣から生じる生活習慣病であり、アルコール性・非アルコール性のいずれにも見られる。近年、肥満に伴うメタボリック症候群が注目されているが、過</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>九竜半島の南半分を「一国二制度」のもとに返還した。返還される以前の中国の行政区分を現代的に再編し、新しい行政区分である特別行政区となった。
+No.3 Ms. Kate Wong (ケティ・ウォン)さん – 2008/12/</t>
+  </si>
+  <si>
+    <t>九竜半島の南半分を「一国二制度」のもとに返還した。返還される以前の中国の行政区分を現代的に再編し、新しい行政区分である特別行政区となった。
+No.3 Ms. Kate Wong (ケティ・ウォン)さん – 2008/12/</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>「新しい仲間」「友の仲間」です。
+■3. 第6回 「音楽会・演奏会のお知らせ」(2018年10月~2019年2月)Check!□第6回 日本ジャンボリー、アフリカ難民救済コンサート、チャリティーイベント等を開催します。■4. 新入会員の募集について(</t>
+  </si>
+  <si>
+    <t>「新しい仲間」「友の仲間」です。
+■3. 第6回 「音楽会・演奏会のお知らせ」(2018年10月~2019年2月)Check!□第6回 日本ジャンボリー、アフリカ難民救済コンサート、チャリティーイベント等を開催します。■4. 新入会員の募集について(</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>約75億人です。
+Q: 現在の経済水準を2.0%ポイント以上改善させるためには何が必要か?</t>
+  </si>
+  <si>
+    <t>約75億人です。
+Q: 現在の経済水準を2.0%ポイント以上改善させるためには何が必要か?</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>「白寿(はくじゅ)」といいます。おめでたい席では、「十回生年月○月○日卒」(じゅっかいねんげつがつび)と読むこともあります。
+Q:9×9=81の句を詠んだ俳人の名前は何さんですか?</t>
+  </si>
+  <si>
+    <t>「白寿(はくじゅ)」といいます。おめでたい席では、「十回生年月○月○日卒」(じゅっかいねんげつがつび)と読むこともあります。
+Q:9×9=81の句を詠んだ俳人の名前は何さんですか?</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>「ゾロアスター教」(別名 : 天地創造の宗教)です。
+【正解】1と2は『コーシン』3は『アケメネス朝ペルシャ』4は『キリスト教・イスラム教』5は『仏教・密教』</t>
+  </si>
+  <si>
+    <t>「ゾロアスター教」(別名 : 天地創造の宗教)です。
+【正解】1と2は『コーシン』3は『アケメネス朝ペルシャ』4は『キリスト教・イスラム教』5は『仏教・密教』</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>cyberagent/open-calm-7b による回答</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>cyberagent/open-calm-7b 正誤</t>
+    <rPh sb="1" eb="3">
+      <t xml:space="preserve">セイゴ </t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -594,6 +743,33 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Hiragino Kaku Gothic ProN"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1020,12 +1196,27 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1382,9 +1573,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1393,11 +1584,14 @@
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="71" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="77.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="42">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="63">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1414,10 +1608,22 @@
         <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="189">
+      <c r="H1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="168">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1433,11 +1639,23 @@
       <c r="E2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="126">
+      <c r="H2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="126">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1453,11 +1671,21 @@
       <c r="E3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="126">
+      <c r="H3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="105">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1473,11 +1701,23 @@
       <c r="E4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="378">
+      <c r="H4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="378">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1493,11 +1733,23 @@
       <c r="E5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="168">
+      <c r="H5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="168">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1513,11 +1765,23 @@
       <c r="E6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="147">
+      <c r="H6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="147">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1533,11 +1797,23 @@
       <c r="E7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="147">
+      <c r="H7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="126">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1553,11 +1829,23 @@
       <c r="E8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="63">
+      <c r="H8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="63">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1573,11 +1861,23 @@
       <c r="E9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="252">
+      <c r="H9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="252">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1593,11 +1893,23 @@
       <c r="E10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="147">
+      <c r="H10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="147">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1613,11 +1925,21 @@
       <c r="E11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="409.6">
+      <c r="H11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="409.6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1633,11 +1955,23 @@
       <c r="E12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="189">
+      <c r="H12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="189">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1653,11 +1987,23 @@
       <c r="E13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="409.6">
+      <c r="H13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="408" customHeight="1">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1673,11 +2019,23 @@
       <c r="E14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="315">
+      <c r="H14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="273">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1693,11 +2051,23 @@
       <c r="E15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="294">
+      <c r="H15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="273">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1713,11 +2083,23 @@
       <c r="E16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="105">
+      <c r="H16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="147">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1733,11 +2115,23 @@
       <c r="E17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="231">
+      <c r="H17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="231">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1753,11 +2147,23 @@
       <c r="E18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="210">
+      <c r="H18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="189">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1773,11 +2179,23 @@
       <c r="E19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="210">
+      <c r="H19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="210">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1793,11 +2211,21 @@
       <c r="E20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="273">
+      <c r="H20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="231">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1813,11 +2241,23 @@
       <c r="E21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="84">
+      <c r="H21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="84">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1833,11 +2273,23 @@
       <c r="E22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="357">
+      <c r="H22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="357">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1853,11 +2305,21 @@
       <c r="E23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="147">
+      <c r="H23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="147">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1873,11 +2335,23 @@
       <c r="E24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="210">
+      <c r="H24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="189">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1893,11 +2367,23 @@
       <c r="E25" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="210">
+      <c r="H25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="189">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1913,12 +2399,259 @@
       <c r="E26" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8D2E64-1146-B445-9B00-36003723FEE7}">
+  <dimension ref="A2:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="1" width="157.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" ht="56" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="42">
+      <c r="A4" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="42">
+      <c r="A9" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="63">
+      <c r="A10" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="42">
+      <c r="A13" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="63">
+      <c r="A16" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="84">
+      <c r="A17" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="42">
+      <c r="A25" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B51D1B0-0408-554B-9EF8-723098A78CA8}">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A1:A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>